<commit_message>
Update Variables in PHS data downloads.xlsx
</commit_message>
<xml_diff>
--- a/data/Variables in PHS data downloads.xlsx
+++ b/data/Variables in PHS data downloads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Malcolm\CodeClan\codeclan_group_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4C1E8A-883F-403C-84EE-8793D3CD36BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83947D98-8C3F-4088-87DA-6A001318EDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="14746" xr2:uid="{1D18E3A5-2E22-425D-8F03-84FC080A4DA4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="81">
   <si>
     <t>_id</t>
   </si>
@@ -250,6 +250,24 @@
   </si>
   <si>
     <t>Hospital activity and patient demographics</t>
+  </si>
+  <si>
+    <t>SIMDQuintile</t>
+  </si>
+  <si>
+    <t>Covid admissions by health board and deprivation</t>
+  </si>
+  <si>
+    <t>AgeGroup</t>
+  </si>
+  <si>
+    <t>AgeGroupQF</t>
+  </si>
+  <si>
+    <t>SexQF</t>
+  </si>
+  <si>
+    <t>Covid admissions by health board, age and sex</t>
   </si>
 </sst>
 </file>
@@ -613,51 +631,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB64AFE-8CE5-449F-BC3C-9578404FFAD8}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -669,16 +695,22 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -693,15 +725,21 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -716,15 +754,21 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -739,15 +783,21 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -762,15 +812,21 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -785,15 +841,21 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -808,18 +870,24 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -828,21 +896,27 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -851,67 +925,82 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>35</v>
       </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>73</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -920,18 +1009,21 @@
         <v>24</v>
       </c>
       <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -940,18 +1032,21 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -960,18 +1055,18 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -980,136 +1075,136 @@
         <v>27</v>
       </c>
       <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="G16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
       </c>
       <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
       </c>
       <c r="D18" t="s">
         <v>68</v>
       </c>
       <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="G18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>69</v>
       </c>
       <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="G19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
       </c>
       <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
         <v>18</v>
       </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="G21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G23" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Delayed discharge data update
</commit_message>
<xml_diff>
--- a/data/Variables in PHS data downloads.xlsx
+++ b/data/Variables in PHS data downloads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Malcolm\CodeClan\codeclan_group_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F1EF04-DA20-4128-AA58-41EA1DA23CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724421FC-2AE4-4C4A-8DC8-B7972F980843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="14746" xr2:uid="{1D18E3A5-2E22-425D-8F03-84FC080A4DA4}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>